<commit_message>
DB modellek + Repok, Gant dia update - VHB
</commit_message>
<xml_diff>
--- a/Documentation/Gantt_dia.xlsx
+++ b/Documentation/Gantt_dia.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\egyetem\3_felev\evp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programok\2021\Git\EVP_Project\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A03828F-1CEE-4C98-879B-5A73342EA28E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6E0989-E362-4972-981E-E2C4BB499CE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">ProjectSchedule!$4:$6</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">ProjectSchedule!$1:$45</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">ProjectSchedule!$1:$47</definedName>
     <definedName name="task_end" localSheetId="0">ProjectSchedule!$F1</definedName>
     <definedName name="task_progress" localSheetId="0">ProjectSchedule!$D1</definedName>
     <definedName name="task_start" localSheetId="0">ProjectSchedule!$E1</definedName>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
   <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
@@ -210,9 +210,6 @@
     <t>RK, HM</t>
   </si>
   <si>
-    <t>HM</t>
-  </si>
-  <si>
     <t>1.mérföldkő - felkészülés</t>
   </si>
   <si>
@@ -268,6 +265,12 @@
   </si>
   <si>
     <t>Várható ZH hét, tanulási szünet</t>
+  </si>
+  <si>
+    <t>Bemutató diagrammok</t>
+  </si>
+  <si>
+    <t>Demo project</t>
   </si>
 </sst>
 </file>
@@ -1051,47 +1054,47 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="17" borderId="2" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="17" borderId="2" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="16" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="16" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="17" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="17" borderId="2" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="17" borderId="2" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="16" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="16" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="17" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1651,11 +1654,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CU49"/>
+  <dimension ref="A1:CU51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
+      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1685,27 +1688,27 @@
       <c r="F1" s="97"/>
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
-      <c r="J1" s="102" t="str">
+      <c r="J1" s="115" t="str">
         <f>HYPERLINK("https://vertex42.link/HowToMakeAGanttChart","► Watch How to Make a Gantt Chart in Excel")</f>
         <v>► Watch How to Make a Gantt Chart in Excel</v>
       </c>
-      <c r="K1" s="102"/>
-      <c r="L1" s="102"/>
-      <c r="M1" s="102"/>
-      <c r="N1" s="102"/>
-      <c r="O1" s="102"/>
-      <c r="P1" s="102"/>
-      <c r="Q1" s="102"/>
-      <c r="R1" s="102"/>
-      <c r="S1" s="102"/>
-      <c r="T1" s="102"/>
-      <c r="U1" s="102"/>
-      <c r="V1" s="102"/>
-      <c r="W1" s="102"/>
-      <c r="X1" s="102"/>
-      <c r="Y1" s="102"/>
-      <c r="Z1" s="102"/>
-      <c r="AA1" s="102"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
     </row>
     <row r="2" spans="1:99" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
@@ -1714,10 +1717,10 @@
       <c r="D2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="106">
+      <c r="E2" s="113">
         <v>44821</v>
       </c>
-      <c r="F2" s="107"/>
+      <c r="F2" s="114"/>
     </row>
     <row r="3" spans="1:99" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
@@ -1726,11 +1729,11 @@
       <c r="D3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="106">
+      <c r="E3" s="113">
         <f ca="1">TODAY()</f>
-        <v>44854</v>
-      </c>
-      <c r="F3" s="107"/>
+        <v>44867</v>
+      </c>
+      <c r="F3" s="114"/>
     </row>
     <row r="4" spans="1:99" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="6" t="s">
@@ -1739,136 +1742,136 @@
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="103">
+      <c r="I4" s="110">
         <f>I5</f>
         <v>44816</v>
       </c>
-      <c r="J4" s="104"/>
-      <c r="K4" s="104"/>
-      <c r="L4" s="104"/>
-      <c r="M4" s="104"/>
-      <c r="N4" s="104"/>
-      <c r="O4" s="105"/>
-      <c r="P4" s="103">
+      <c r="J4" s="111"/>
+      <c r="K4" s="111"/>
+      <c r="L4" s="111"/>
+      <c r="M4" s="111"/>
+      <c r="N4" s="111"/>
+      <c r="O4" s="112"/>
+      <c r="P4" s="110">
         <f>P5</f>
         <v>44823</v>
       </c>
-      <c r="Q4" s="104"/>
-      <c r="R4" s="104"/>
-      <c r="S4" s="104"/>
-      <c r="T4" s="104"/>
-      <c r="U4" s="104"/>
-      <c r="V4" s="105"/>
-      <c r="W4" s="103">
+      <c r="Q4" s="111"/>
+      <c r="R4" s="111"/>
+      <c r="S4" s="111"/>
+      <c r="T4" s="111"/>
+      <c r="U4" s="111"/>
+      <c r="V4" s="112"/>
+      <c r="W4" s="110">
         <f>W5</f>
         <v>44830</v>
       </c>
-      <c r="X4" s="104"/>
-      <c r="Y4" s="104"/>
-      <c r="Z4" s="104"/>
-      <c r="AA4" s="104"/>
-      <c r="AB4" s="104"/>
-      <c r="AC4" s="105"/>
-      <c r="AD4" s="103">
+      <c r="X4" s="111"/>
+      <c r="Y4" s="111"/>
+      <c r="Z4" s="111"/>
+      <c r="AA4" s="111"/>
+      <c r="AB4" s="111"/>
+      <c r="AC4" s="112"/>
+      <c r="AD4" s="110">
         <f>AD5</f>
         <v>44837</v>
       </c>
-      <c r="AE4" s="104"/>
-      <c r="AF4" s="104"/>
-      <c r="AG4" s="104"/>
-      <c r="AH4" s="104"/>
-      <c r="AI4" s="104"/>
-      <c r="AJ4" s="105"/>
-      <c r="AK4" s="103">
+      <c r="AE4" s="111"/>
+      <c r="AF4" s="111"/>
+      <c r="AG4" s="111"/>
+      <c r="AH4" s="111"/>
+      <c r="AI4" s="111"/>
+      <c r="AJ4" s="112"/>
+      <c r="AK4" s="110">
         <f>AK5</f>
         <v>44844</v>
       </c>
-      <c r="AL4" s="104"/>
-      <c r="AM4" s="104"/>
-      <c r="AN4" s="104"/>
-      <c r="AO4" s="104"/>
-      <c r="AP4" s="104"/>
-      <c r="AQ4" s="105"/>
-      <c r="AR4" s="103">
+      <c r="AL4" s="111"/>
+      <c r="AM4" s="111"/>
+      <c r="AN4" s="111"/>
+      <c r="AO4" s="111"/>
+      <c r="AP4" s="111"/>
+      <c r="AQ4" s="112"/>
+      <c r="AR4" s="110">
         <f>AR5</f>
         <v>44851</v>
       </c>
-      <c r="AS4" s="104"/>
-      <c r="AT4" s="104"/>
-      <c r="AU4" s="104"/>
-      <c r="AV4" s="104"/>
-      <c r="AW4" s="104"/>
-      <c r="AX4" s="105"/>
-      <c r="AY4" s="103">
+      <c r="AS4" s="111"/>
+      <c r="AT4" s="111"/>
+      <c r="AU4" s="111"/>
+      <c r="AV4" s="111"/>
+      <c r="AW4" s="111"/>
+      <c r="AX4" s="112"/>
+      <c r="AY4" s="110">
         <f>AY5</f>
         <v>44858</v>
       </c>
-      <c r="AZ4" s="104"/>
-      <c r="BA4" s="104"/>
-      <c r="BB4" s="104"/>
-      <c r="BC4" s="104"/>
-      <c r="BD4" s="104"/>
-      <c r="BE4" s="105"/>
-      <c r="BF4" s="103">
+      <c r="AZ4" s="111"/>
+      <c r="BA4" s="111"/>
+      <c r="BB4" s="111"/>
+      <c r="BC4" s="111"/>
+      <c r="BD4" s="111"/>
+      <c r="BE4" s="112"/>
+      <c r="BF4" s="110">
         <f>BF5</f>
         <v>44865</v>
       </c>
-      <c r="BG4" s="104"/>
-      <c r="BH4" s="104"/>
-      <c r="BI4" s="104"/>
-      <c r="BJ4" s="104"/>
-      <c r="BK4" s="104"/>
-      <c r="BL4" s="105"/>
-      <c r="BM4" s="103">
+      <c r="BG4" s="111"/>
+      <c r="BH4" s="111"/>
+      <c r="BI4" s="111"/>
+      <c r="BJ4" s="111"/>
+      <c r="BK4" s="111"/>
+      <c r="BL4" s="112"/>
+      <c r="BM4" s="110">
         <f>BM5</f>
         <v>44872</v>
       </c>
-      <c r="BN4" s="104"/>
-      <c r="BO4" s="104"/>
-      <c r="BP4" s="104"/>
-      <c r="BQ4" s="104"/>
-      <c r="BR4" s="104"/>
-      <c r="BS4" s="105"/>
-      <c r="BT4" s="103">
+      <c r="BN4" s="111"/>
+      <c r="BO4" s="111"/>
+      <c r="BP4" s="111"/>
+      <c r="BQ4" s="111"/>
+      <c r="BR4" s="111"/>
+      <c r="BS4" s="112"/>
+      <c r="BT4" s="110">
         <f>BT5</f>
         <v>44879</v>
       </c>
-      <c r="BU4" s="104"/>
-      <c r="BV4" s="104"/>
-      <c r="BW4" s="104"/>
-      <c r="BX4" s="104"/>
-      <c r="BY4" s="104"/>
-      <c r="BZ4" s="105"/>
-      <c r="CA4" s="103">
+      <c r="BU4" s="111"/>
+      <c r="BV4" s="111"/>
+      <c r="BW4" s="111"/>
+      <c r="BX4" s="111"/>
+      <c r="BY4" s="111"/>
+      <c r="BZ4" s="112"/>
+      <c r="CA4" s="110">
         <f>CA5</f>
         <v>44886</v>
       </c>
-      <c r="CB4" s="104"/>
-      <c r="CC4" s="104"/>
-      <c r="CD4" s="104"/>
-      <c r="CE4" s="104"/>
-      <c r="CF4" s="104"/>
-      <c r="CG4" s="105"/>
-      <c r="CH4" s="103">
+      <c r="CB4" s="111"/>
+      <c r="CC4" s="111"/>
+      <c r="CD4" s="111"/>
+      <c r="CE4" s="111"/>
+      <c r="CF4" s="111"/>
+      <c r="CG4" s="112"/>
+      <c r="CH4" s="110">
         <f>CH5</f>
         <v>44893</v>
       </c>
-      <c r="CI4" s="104"/>
-      <c r="CJ4" s="104"/>
-      <c r="CK4" s="104"/>
-      <c r="CL4" s="104"/>
-      <c r="CM4" s="104"/>
-      <c r="CN4" s="105"/>
-      <c r="CO4" s="103">
+      <c r="CI4" s="111"/>
+      <c r="CJ4" s="111"/>
+      <c r="CK4" s="111"/>
+      <c r="CL4" s="111"/>
+      <c r="CM4" s="111"/>
+      <c r="CN4" s="112"/>
+      <c r="CO4" s="110">
         <f>CO5</f>
         <v>44900</v>
       </c>
-      <c r="CP4" s="104"/>
-      <c r="CQ4" s="104"/>
-      <c r="CR4" s="104"/>
-      <c r="CS4" s="104"/>
-      <c r="CT4" s="104"/>
-      <c r="CU4" s="105"/>
+      <c r="CP4" s="111"/>
+      <c r="CQ4" s="111"/>
+      <c r="CR4" s="111"/>
+      <c r="CS4" s="111"/>
+      <c r="CT4" s="111"/>
+      <c r="CU4" s="112"/>
     </row>
     <row r="5" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
@@ -2150,7 +2153,7 @@
         <v>44884</v>
       </c>
       <c r="BZ5" s="14">
-        <f t="shared" ref="BZ5:CB5" si="12">BY5+1</f>
+        <f t="shared" ref="BZ5" si="12">BY5+1</f>
         <v>44885</v>
       </c>
       <c r="CA5" s="13">
@@ -2568,7 +2571,7 @@
         <v>d</v>
       </c>
       <c r="CH6" s="15" t="str">
-        <f t="shared" ref="CH6:DI6" si="33">LEFT(TEXT(CH5,"ddd"),1)</f>
+        <f t="shared" ref="CH6:CN6" si="33">LEFT(TEXT(CH5,"ddd"),1)</f>
         <v>d</v>
       </c>
       <c r="CI6" s="15" t="str">
@@ -2633,7 +2636,7 @@
       <c r="F7" s="24"/>
       <c r="G7" s="25"/>
       <c r="H7" s="25" t="str">
-        <f t="shared" ref="H7:H45" si="35">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H7:H47" si="35">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I7" s="81"/>
@@ -2731,7 +2734,7 @@
     <row r="8" spans="1:99" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19"/>
       <c r="B8" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="27"/>
       <c r="D8" s="28"/>
@@ -3185,7 +3188,7 @@
         <v>39</v>
       </c>
       <c r="D12" s="33">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="E12" s="34">
         <v>44828</v>
@@ -3407,7 +3410,7 @@
     <row r="14" spans="1:99" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19"/>
       <c r="B14" s="35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="36"/>
       <c r="D14" s="37"/>
@@ -3747,7 +3750,7 @@
         <v>42</v>
       </c>
       <c r="D17" s="42">
-        <v>0.85</v>
+        <v>0.99</v>
       </c>
       <c r="E17" s="43">
         <v>44849</v>
@@ -3861,7 +3864,7 @@
         <v>39</v>
       </c>
       <c r="D18" s="42">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E18" s="43">
         <v>44828</v>
@@ -4185,7 +4188,7 @@
         <v>42</v>
       </c>
       <c r="D21" s="52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="53">
         <v>44856</v>
@@ -4413,7 +4416,7 @@
         <v>45</v>
       </c>
       <c r="D23" s="52">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E23" s="53">
         <v>44864</v>
@@ -4527,7 +4530,7 @@
         <v>42</v>
       </c>
       <c r="D24" s="52">
-        <v>0</v>
+        <v>0.99</v>
       </c>
       <c r="E24" s="53">
         <v>44862</v>
@@ -4635,25 +4638,22 @@
     <row r="25" spans="1:99" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
       <c r="B25" s="50" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="C25" s="51" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D25" s="52">
-        <v>0</v>
+        <v>0.99</v>
       </c>
       <c r="E25" s="53">
         <v>44862</v>
       </c>
       <c r="F25" s="53">
-        <v>44864</v>
+        <v>44868</v>
       </c>
       <c r="G25" s="25"/>
-      <c r="H25" s="25">
-        <f t="shared" si="35"/>
-        <v>3</v>
-      </c>
+      <c r="H25" s="25"/>
       <c r="I25" s="81"/>
       <c r="J25" s="81"/>
       <c r="K25" s="81"/>
@@ -4749,19 +4749,19 @@
     <row r="26" spans="1:99" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="50" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C26" s="51" t="s">
         <v>39</v>
       </c>
       <c r="D26" s="52">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="E26" s="53">
-        <v>44851</v>
-      </c>
-      <c r="F26" s="54">
-        <v>44862</v>
+        <v>44855</v>
+      </c>
+      <c r="F26" s="53">
+        <v>44868</v>
       </c>
       <c r="G26" s="25"/>
       <c r="H26" s="25"/>
@@ -4859,17 +4859,25 @@
     </row>
     <row r="27" spans="1:99" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
-      <c r="B27" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="56"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="59"/>
+      <c r="B27" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="52">
+        <v>0.99</v>
+      </c>
+      <c r="E27" s="53">
+        <v>44862</v>
+      </c>
+      <c r="F27" s="53">
+        <v>44864</v>
+      </c>
       <c r="G27" s="25"/>
-      <c r="H27" s="25" t="str">
+      <c r="H27" s="25">
         <f t="shared" si="35"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="I27" s="81"/>
       <c r="J27" s="81"/>
@@ -4965,26 +4973,23 @@
     </row>
     <row r="28" spans="1:99" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="19"/>
-      <c r="B28" s="60" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="61" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="62">
-        <v>0</v>
-      </c>
-      <c r="E28" s="63">
-        <v>44869</v>
-      </c>
-      <c r="F28" s="63">
-        <v>44871</v>
+      <c r="B28" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="52">
+        <v>1</v>
+      </c>
+      <c r="E28" s="53">
+        <v>44851</v>
+      </c>
+      <c r="F28" s="54">
+        <v>44862</v>
       </c>
       <c r="G28" s="25"/>
-      <c r="H28" s="25">
-        <f t="shared" si="35"/>
-        <v>3</v>
-      </c>
+      <c r="H28" s="25"/>
       <c r="I28" s="81"/>
       <c r="J28" s="81"/>
       <c r="K28" s="81"/>
@@ -5079,25 +5084,17 @@
     </row>
     <row r="29" spans="1:99" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="19"/>
-      <c r="B29" s="60" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="61" t="s">
-        <v>45</v>
-      </c>
-      <c r="D29" s="62">
-        <v>0</v>
-      </c>
-      <c r="E29" s="63">
-        <v>44871</v>
-      </c>
-      <c r="F29" s="63">
-        <v>44876</v>
-      </c>
+      <c r="B29" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="56"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="59"/>
       <c r="G29" s="25"/>
-      <c r="H29" s="25">
+      <c r="H29" s="25" t="str">
         <f t="shared" si="35"/>
-        <v>6</v>
+        <v/>
       </c>
       <c r="I29" s="81"/>
       <c r="J29" s="81"/>
@@ -5194,10 +5191,10 @@
     <row r="30" spans="1:99" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="19"/>
       <c r="B30" s="60" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C30" s="61" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D30" s="62">
         <v>0</v>
@@ -5206,12 +5203,12 @@
         <v>44869</v>
       </c>
       <c r="F30" s="63">
-        <v>44874</v>
+        <v>44871</v>
       </c>
       <c r="G30" s="25"/>
       <c r="H30" s="25">
         <f t="shared" si="35"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I30" s="81"/>
       <c r="J30" s="81"/>
@@ -5308,16 +5305,16 @@
     <row r="31" spans="1:99" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="19"/>
       <c r="B31" s="60" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C31" s="61" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D31" s="62">
         <v>0</v>
       </c>
       <c r="E31" s="63">
-        <v>44874</v>
+        <v>44871</v>
       </c>
       <c r="F31" s="63">
         <v>44876</v>
@@ -5325,7 +5322,7 @@
       <c r="G31" s="25"/>
       <c r="H31" s="25">
         <f t="shared" si="35"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I31" s="81"/>
       <c r="J31" s="81"/>
@@ -5421,15 +5418,25 @@
     </row>
     <row r="32" spans="1:99" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="19"/>
-      <c r="B32" s="60"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="62"/>
-      <c r="E32" s="63"/>
-      <c r="F32" s="64"/>
+      <c r="B32" s="60" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="61" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="62">
+        <v>0</v>
+      </c>
+      <c r="E32" s="63">
+        <v>44869</v>
+      </c>
+      <c r="F32" s="63">
+        <v>44874</v>
+      </c>
       <c r="G32" s="25"/>
-      <c r="H32" s="25" t="str">
+      <c r="H32" s="25">
         <f t="shared" si="35"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="I32" s="81"/>
       <c r="J32" s="81"/>
@@ -5525,17 +5532,25 @@
     </row>
     <row r="33" spans="1:99" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="19"/>
-      <c r="B33" s="65" t="s">
-        <v>54</v>
-      </c>
-      <c r="C33" s="66"/>
-      <c r="D33" s="67"/>
-      <c r="E33" s="68"/>
-      <c r="F33" s="69"/>
+      <c r="B33" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="61" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="62">
+        <v>0</v>
+      </c>
+      <c r="E33" s="63">
+        <v>44874</v>
+      </c>
+      <c r="F33" s="63">
+        <v>44876</v>
+      </c>
       <c r="G33" s="25"/>
-      <c r="H33" s="25" t="str">
+      <c r="H33" s="25">
         <f t="shared" si="35"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="I33" s="81"/>
       <c r="J33" s="81"/>
@@ -5631,25 +5646,15 @@
     </row>
     <row r="34" spans="1:99" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="19"/>
-      <c r="B34" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="C34" s="71" t="s">
-        <v>41</v>
-      </c>
-      <c r="D34" s="72">
-        <v>0</v>
-      </c>
-      <c r="E34" s="73">
-        <v>44876</v>
-      </c>
-      <c r="F34" s="74">
-        <v>44878</v>
-      </c>
+      <c r="B34" s="60"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="62"/>
+      <c r="E34" s="63"/>
+      <c r="F34" s="64"/>
       <c r="G34" s="25"/>
-      <c r="H34" s="25">
+      <c r="H34" s="25" t="str">
         <f t="shared" si="35"/>
-        <v>3</v>
+        <v/>
       </c>
       <c r="I34" s="81"/>
       <c r="J34" s="81"/>
@@ -5745,25 +5750,17 @@
     </row>
     <row r="35" spans="1:99" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="19"/>
-      <c r="B35" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" s="71" t="s">
-        <v>45</v>
-      </c>
-      <c r="D35" s="72">
-        <v>0</v>
-      </c>
-      <c r="E35" s="73">
-        <v>44878</v>
-      </c>
-      <c r="F35" s="74">
-        <v>44883</v>
-      </c>
+      <c r="B35" s="65" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="66"/>
+      <c r="D35" s="67"/>
+      <c r="E35" s="68"/>
+      <c r="F35" s="69"/>
       <c r="G35" s="25"/>
-      <c r="H35" s="25">
+      <c r="H35" s="25" t="str">
         <f t="shared" si="35"/>
-        <v>6</v>
+        <v/>
       </c>
       <c r="I35" s="81"/>
       <c r="J35" s="81"/>
@@ -5860,10 +5857,10 @@
     <row r="36" spans="1:99" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="19"/>
       <c r="B36" s="70" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C36" s="71" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D36" s="72">
         <v>0</v>
@@ -5872,12 +5869,12 @@
         <v>44876</v>
       </c>
       <c r="F36" s="74">
-        <v>44883</v>
+        <v>44878</v>
       </c>
       <c r="G36" s="25"/>
       <c r="H36" s="25">
         <f t="shared" si="35"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I36" s="81"/>
       <c r="J36" s="81"/>
@@ -5974,24 +5971,24 @@
     <row r="37" spans="1:99" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="19"/>
       <c r="B37" s="70" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C37" s="71" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D37" s="72">
         <v>0</v>
       </c>
       <c r="E37" s="73">
+        <v>44878</v>
+      </c>
+      <c r="F37" s="74">
         <v>44883</v>
-      </c>
-      <c r="F37" s="73">
-        <v>44889</v>
       </c>
       <c r="G37" s="25"/>
       <c r="H37" s="25">
         <f t="shared" si="35"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I37" s="81"/>
       <c r="J37" s="81"/>
@@ -6088,24 +6085,24 @@
     <row r="38" spans="1:99" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="19"/>
       <c r="B38" s="70" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C38" s="71" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D38" s="72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38" s="73">
-        <v>44890</v>
+        <v>44876</v>
       </c>
       <c r="F38" s="74">
-        <v>44896</v>
+        <v>44883</v>
       </c>
       <c r="G38" s="25"/>
       <c r="H38" s="25">
         <f t="shared" si="35"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I38" s="81"/>
       <c r="J38" s="81"/>
@@ -6201,17 +6198,25 @@
     </row>
     <row r="39" spans="1:99" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="19"/>
-      <c r="B39" s="115" t="s">
-        <v>59</v>
-      </c>
-      <c r="C39" s="108"/>
-      <c r="D39" s="109"/>
-      <c r="E39" s="110"/>
-      <c r="F39" s="110"/>
+      <c r="B39" s="70" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="71" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" s="72">
+        <v>0</v>
+      </c>
+      <c r="E39" s="73">
+        <v>44883</v>
+      </c>
+      <c r="F39" s="73">
+        <v>44889</v>
+      </c>
       <c r="G39" s="25"/>
-      <c r="H39" s="25" t="str">
+      <c r="H39" s="25">
         <f t="shared" si="35"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="I39" s="81"/>
       <c r="J39" s="81"/>
@@ -6307,23 +6312,26 @@
     </row>
     <row r="40" spans="1:99" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="19"/>
-      <c r="B40" s="111" t="s">
-        <v>60</v>
-      </c>
-      <c r="C40" s="112" t="s">
-        <v>41</v>
-      </c>
-      <c r="D40" s="113">
-        <v>0</v>
-      </c>
-      <c r="E40" s="114">
+      <c r="B40" s="70" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" s="71" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" s="72">
+        <v>1</v>
+      </c>
+      <c r="E40" s="73">
+        <v>44890</v>
+      </c>
+      <c r="F40" s="74">
         <v>44896</v>
       </c>
-      <c r="F40" s="114">
-        <v>44898</v>
-      </c>
       <c r="G40" s="25"/>
-      <c r="H40" s="25"/>
+      <c r="H40" s="25">
+        <f t="shared" si="35"/>
+        <v>7</v>
+      </c>
       <c r="I40" s="81"/>
       <c r="J40" s="81"/>
       <c r="K40" s="81"/>
@@ -6418,23 +6426,18 @@
     </row>
     <row r="41" spans="1:99" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="19"/>
-      <c r="B41" s="111" t="s">
-        <v>61</v>
-      </c>
-      <c r="C41" s="112" t="s">
-        <v>45</v>
-      </c>
-      <c r="D41" s="113">
-        <v>0</v>
-      </c>
-      <c r="E41" s="114">
-        <v>44898</v>
-      </c>
-      <c r="F41" s="114">
-        <v>44901</v>
-      </c>
+      <c r="B41" s="109" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" s="102"/>
+      <c r="D41" s="103"/>
+      <c r="E41" s="104"/>
+      <c r="F41" s="104"/>
       <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
+      <c r="H41" s="25" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
       <c r="I41" s="81"/>
       <c r="J41" s="81"/>
       <c r="K41" s="81"/>
@@ -6529,19 +6532,19 @@
     </row>
     <row r="42" spans="1:99" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="19"/>
-      <c r="B42" s="111" t="s">
-        <v>62</v>
-      </c>
-      <c r="C42" s="112" t="s">
-        <v>42</v>
-      </c>
-      <c r="D42" s="113">
+      <c r="B42" s="105" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="106" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42" s="107">
         <v>0</v>
       </c>
-      <c r="E42" s="114">
+      <c r="E42" s="108">
         <v>44896</v>
       </c>
-      <c r="F42" s="114">
+      <c r="F42" s="108">
         <v>44898</v>
       </c>
       <c r="G42" s="25"/>
@@ -6640,26 +6643,23 @@
     </row>
     <row r="43" spans="1:99" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="19"/>
-      <c r="B43" s="111" t="s">
-        <v>63</v>
-      </c>
-      <c r="C43" s="112" t="s">
-        <v>42</v>
-      </c>
-      <c r="D43" s="113">
+      <c r="B43" s="105" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" s="106" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" s="107">
         <v>0</v>
       </c>
-      <c r="E43" s="114">
+      <c r="E43" s="108">
         <v>44898</v>
       </c>
-      <c r="F43" s="114">
+      <c r="F43" s="108">
         <v>44901</v>
       </c>
       <c r="G43" s="25"/>
-      <c r="H43" s="25">
-        <f t="shared" si="35"/>
-        <v>4</v>
-      </c>
+      <c r="H43" s="25"/>
       <c r="I43" s="81"/>
       <c r="J43" s="81"/>
       <c r="K43" s="81"/>
@@ -6754,16 +6754,23 @@
     </row>
     <row r="44" spans="1:99" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="19"/>
-      <c r="B44" s="111"/>
-      <c r="C44" s="112"/>
-      <c r="D44" s="113"/>
-      <c r="E44" s="114"/>
-      <c r="F44" s="114"/>
+      <c r="B44" s="105" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" s="106" t="s">
+        <v>42</v>
+      </c>
+      <c r="D44" s="107">
+        <v>0</v>
+      </c>
+      <c r="E44" s="108">
+        <v>44896</v>
+      </c>
+      <c r="F44" s="108">
+        <v>44898</v>
+      </c>
       <c r="G44" s="25"/>
-      <c r="H44" s="25" t="str">
-        <f t="shared" si="35"/>
-        <v/>
-      </c>
+      <c r="H44" s="25"/>
       <c r="I44" s="81"/>
       <c r="J44" s="81"/>
       <c r="K44" s="81"/>
@@ -6858,154 +6865,372 @@
     </row>
     <row r="45" spans="1:99" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="19"/>
-      <c r="B45" s="75" t="s">
+      <c r="B45" s="105" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" s="106" t="s">
+        <v>42</v>
+      </c>
+      <c r="D45" s="107">
         <v>0</v>
       </c>
-      <c r="C45" s="76"/>
-      <c r="D45" s="77"/>
-      <c r="E45" s="78"/>
-      <c r="F45" s="79"/>
-      <c r="G45" s="80"/>
-      <c r="H45" s="80" t="str">
+      <c r="E45" s="108">
+        <v>44898</v>
+      </c>
+      <c r="F45" s="108">
+        <v>44901</v>
+      </c>
+      <c r="G45" s="25"/>
+      <c r="H45" s="25">
+        <f t="shared" si="35"/>
+        <v>4</v>
+      </c>
+      <c r="I45" s="81"/>
+      <c r="J45" s="81"/>
+      <c r="K45" s="81"/>
+      <c r="L45" s="81"/>
+      <c r="M45" s="81"/>
+      <c r="N45" s="81"/>
+      <c r="O45" s="81"/>
+      <c r="P45" s="81"/>
+      <c r="Q45" s="81"/>
+      <c r="R45" s="81"/>
+      <c r="S45" s="81"/>
+      <c r="T45" s="81"/>
+      <c r="U45" s="81"/>
+      <c r="V45" s="81"/>
+      <c r="W45" s="81"/>
+      <c r="X45" s="81"/>
+      <c r="Y45" s="81"/>
+      <c r="Z45" s="81"/>
+      <c r="AA45" s="81"/>
+      <c r="AB45" s="81"/>
+      <c r="AC45" s="81"/>
+      <c r="AD45" s="81"/>
+      <c r="AE45" s="81"/>
+      <c r="AF45" s="81"/>
+      <c r="AG45" s="81"/>
+      <c r="AH45" s="81"/>
+      <c r="AI45" s="81"/>
+      <c r="AJ45" s="81"/>
+      <c r="AK45" s="81"/>
+      <c r="AL45" s="81"/>
+      <c r="AM45" s="81"/>
+      <c r="AN45" s="81"/>
+      <c r="AO45" s="81"/>
+      <c r="AP45" s="81"/>
+      <c r="AQ45" s="81"/>
+      <c r="AR45" s="81"/>
+      <c r="AS45" s="81"/>
+      <c r="AT45" s="81"/>
+      <c r="AU45" s="81"/>
+      <c r="AV45" s="81"/>
+      <c r="AW45" s="81"/>
+      <c r="AX45" s="81"/>
+      <c r="AY45" s="81"/>
+      <c r="AZ45" s="81"/>
+      <c r="BA45" s="81"/>
+      <c r="BB45" s="81"/>
+      <c r="BC45" s="81"/>
+      <c r="BD45" s="81"/>
+      <c r="BE45" s="81"/>
+      <c r="BF45" s="81"/>
+      <c r="BG45" s="81"/>
+      <c r="BH45" s="81"/>
+      <c r="BI45" s="81"/>
+      <c r="BJ45" s="81"/>
+      <c r="BK45" s="81"/>
+      <c r="BL45" s="81"/>
+      <c r="BM45" s="81"/>
+      <c r="BN45" s="81"/>
+      <c r="BO45" s="81"/>
+      <c r="BP45" s="81"/>
+      <c r="BQ45" s="81"/>
+      <c r="BR45" s="81"/>
+      <c r="BS45" s="81"/>
+      <c r="BT45" s="81"/>
+      <c r="BU45" s="81"/>
+      <c r="BV45" s="81"/>
+      <c r="BW45" s="81"/>
+      <c r="BX45" s="81"/>
+      <c r="BY45" s="81"/>
+      <c r="BZ45" s="81"/>
+      <c r="CA45" s="81"/>
+      <c r="CB45" s="81"/>
+      <c r="CC45" s="81"/>
+      <c r="CD45" s="81"/>
+      <c r="CE45" s="81"/>
+      <c r="CF45" s="81"/>
+      <c r="CG45" s="81"/>
+      <c r="CH45" s="81"/>
+      <c r="CI45" s="81"/>
+      <c r="CJ45" s="81"/>
+      <c r="CK45" s="81"/>
+      <c r="CL45" s="81"/>
+      <c r="CM45" s="81"/>
+      <c r="CN45" s="81"/>
+      <c r="CO45" s="81"/>
+      <c r="CP45" s="81"/>
+      <c r="CQ45" s="81"/>
+      <c r="CR45" s="81"/>
+      <c r="CS45" s="81"/>
+      <c r="CT45" s="81"/>
+      <c r="CU45" s="81"/>
+    </row>
+    <row r="46" spans="1:99" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="19"/>
+      <c r="B46" s="105"/>
+      <c r="C46" s="106"/>
+      <c r="D46" s="107"/>
+      <c r="E46" s="108"/>
+      <c r="F46" s="108"/>
+      <c r="G46" s="25"/>
+      <c r="H46" s="25" t="str">
         <f t="shared" si="35"/>
         <v/>
       </c>
-      <c r="I45" s="83"/>
-      <c r="J45" s="83"/>
-      <c r="K45" s="83"/>
-      <c r="L45" s="83"/>
-      <c r="M45" s="83"/>
-      <c r="N45" s="83"/>
-      <c r="O45" s="83"/>
-      <c r="P45" s="83"/>
-      <c r="Q45" s="83"/>
-      <c r="R45" s="83"/>
-      <c r="S45" s="83"/>
-      <c r="T45" s="83"/>
-      <c r="U45" s="83"/>
-      <c r="V45" s="83"/>
-      <c r="W45" s="83"/>
-      <c r="X45" s="83"/>
-      <c r="Y45" s="83"/>
-      <c r="Z45" s="83"/>
-      <c r="AA45" s="83"/>
-      <c r="AB45" s="83"/>
-      <c r="AC45" s="83"/>
-      <c r="AD45" s="83"/>
-      <c r="AE45" s="83"/>
-      <c r="AF45" s="83"/>
-      <c r="AG45" s="83"/>
-      <c r="AH45" s="83"/>
-      <c r="AI45" s="83"/>
-      <c r="AJ45" s="83"/>
-      <c r="AK45" s="83"/>
-      <c r="AL45" s="83"/>
-      <c r="AM45" s="83"/>
-      <c r="AN45" s="83"/>
-      <c r="AO45" s="83"/>
-      <c r="AP45" s="83"/>
-      <c r="AQ45" s="83"/>
-      <c r="AR45" s="83"/>
-      <c r="AS45" s="83"/>
-      <c r="AT45" s="83"/>
-      <c r="AU45" s="83"/>
-      <c r="AV45" s="83"/>
-      <c r="AW45" s="83"/>
-      <c r="AX45" s="83"/>
-      <c r="AY45" s="83"/>
-      <c r="AZ45" s="83"/>
-      <c r="BA45" s="83"/>
-      <c r="BB45" s="83"/>
-      <c r="BC45" s="83"/>
-      <c r="BD45" s="83"/>
-      <c r="BE45" s="83"/>
-      <c r="BF45" s="83"/>
-      <c r="BG45" s="83"/>
-      <c r="BH45" s="83"/>
-      <c r="BI45" s="83"/>
-      <c r="BJ45" s="83"/>
-      <c r="BK45" s="83"/>
-      <c r="BL45" s="83"/>
-      <c r="BM45" s="83"/>
-      <c r="BN45" s="83"/>
-      <c r="BO45" s="83"/>
-      <c r="BP45" s="83"/>
-      <c r="BQ45" s="83"/>
-      <c r="BR45" s="83"/>
-      <c r="BS45" s="83"/>
-      <c r="BT45" s="83"/>
-      <c r="BU45" s="83"/>
-      <c r="BV45" s="83"/>
-      <c r="BW45" s="83"/>
-      <c r="BX45" s="83"/>
-      <c r="BY45" s="83"/>
-      <c r="BZ45" s="83"/>
-      <c r="CA45" s="83"/>
-      <c r="CB45" s="83"/>
-      <c r="CC45" s="83"/>
-      <c r="CD45" s="83"/>
-      <c r="CE45" s="83"/>
-      <c r="CF45" s="83"/>
-      <c r="CG45" s="83"/>
-      <c r="CH45" s="83"/>
-      <c r="CI45" s="83"/>
-      <c r="CJ45" s="83"/>
-      <c r="CK45" s="83"/>
-      <c r="CL45" s="83"/>
-      <c r="CM45" s="83"/>
-      <c r="CN45" s="83"/>
-      <c r="CO45" s="83"/>
-      <c r="CP45" s="83"/>
-      <c r="CQ45" s="83"/>
-      <c r="CR45" s="83"/>
-      <c r="CS45" s="83"/>
-      <c r="CT45" s="83"/>
-      <c r="CU45" s="83"/>
+      <c r="I46" s="81"/>
+      <c r="J46" s="81"/>
+      <c r="K46" s="81"/>
+      <c r="L46" s="81"/>
+      <c r="M46" s="81"/>
+      <c r="N46" s="81"/>
+      <c r="O46" s="81"/>
+      <c r="P46" s="81"/>
+      <c r="Q46" s="81"/>
+      <c r="R46" s="81"/>
+      <c r="S46" s="81"/>
+      <c r="T46" s="81"/>
+      <c r="U46" s="81"/>
+      <c r="V46" s="81"/>
+      <c r="W46" s="81"/>
+      <c r="X46" s="81"/>
+      <c r="Y46" s="81"/>
+      <c r="Z46" s="81"/>
+      <c r="AA46" s="81"/>
+      <c r="AB46" s="81"/>
+      <c r="AC46" s="81"/>
+      <c r="AD46" s="81"/>
+      <c r="AE46" s="81"/>
+      <c r="AF46" s="81"/>
+      <c r="AG46" s="81"/>
+      <c r="AH46" s="81"/>
+      <c r="AI46" s="81"/>
+      <c r="AJ46" s="81"/>
+      <c r="AK46" s="81"/>
+      <c r="AL46" s="81"/>
+      <c r="AM46" s="81"/>
+      <c r="AN46" s="81"/>
+      <c r="AO46" s="81"/>
+      <c r="AP46" s="81"/>
+      <c r="AQ46" s="81"/>
+      <c r="AR46" s="81"/>
+      <c r="AS46" s="81"/>
+      <c r="AT46" s="81"/>
+      <c r="AU46" s="81"/>
+      <c r="AV46" s="81"/>
+      <c r="AW46" s="81"/>
+      <c r="AX46" s="81"/>
+      <c r="AY46" s="81"/>
+      <c r="AZ46" s="81"/>
+      <c r="BA46" s="81"/>
+      <c r="BB46" s="81"/>
+      <c r="BC46" s="81"/>
+      <c r="BD46" s="81"/>
+      <c r="BE46" s="81"/>
+      <c r="BF46" s="81"/>
+      <c r="BG46" s="81"/>
+      <c r="BH46" s="81"/>
+      <c r="BI46" s="81"/>
+      <c r="BJ46" s="81"/>
+      <c r="BK46" s="81"/>
+      <c r="BL46" s="81"/>
+      <c r="BM46" s="81"/>
+      <c r="BN46" s="81"/>
+      <c r="BO46" s="81"/>
+      <c r="BP46" s="81"/>
+      <c r="BQ46" s="81"/>
+      <c r="BR46" s="81"/>
+      <c r="BS46" s="81"/>
+      <c r="BT46" s="81"/>
+      <c r="BU46" s="81"/>
+      <c r="BV46" s="81"/>
+      <c r="BW46" s="81"/>
+      <c r="BX46" s="81"/>
+      <c r="BY46" s="81"/>
+      <c r="BZ46" s="81"/>
+      <c r="CA46" s="81"/>
+      <c r="CB46" s="81"/>
+      <c r="CC46" s="81"/>
+      <c r="CD46" s="81"/>
+      <c r="CE46" s="81"/>
+      <c r="CF46" s="81"/>
+      <c r="CG46" s="81"/>
+      <c r="CH46" s="81"/>
+      <c r="CI46" s="81"/>
+      <c r="CJ46" s="81"/>
+      <c r="CK46" s="81"/>
+      <c r="CL46" s="81"/>
+      <c r="CM46" s="81"/>
+      <c r="CN46" s="81"/>
+      <c r="CO46" s="81"/>
+      <c r="CP46" s="81"/>
+      <c r="CQ46" s="81"/>
+      <c r="CR46" s="81"/>
+      <c r="CS46" s="81"/>
+      <c r="CT46" s="81"/>
+      <c r="CU46" s="81"/>
     </row>
-    <row r="46" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
-      <c r="G46" s="6"/>
-    </row>
-    <row r="47" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="B47" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C47" s="17"/>
-      <c r="F47" s="96">
-        <v>43113</v>
-      </c>
+    <row r="47" spans="1:99" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="19"/>
+      <c r="B47" s="75" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="76"/>
+      <c r="D47" s="77"/>
+      <c r="E47" s="78"/>
+      <c r="F47" s="79"/>
+      <c r="G47" s="80"/>
+      <c r="H47" s="80" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="I47" s="83"/>
+      <c r="J47" s="83"/>
+      <c r="K47" s="83"/>
+      <c r="L47" s="83"/>
+      <c r="M47" s="83"/>
+      <c r="N47" s="83"/>
+      <c r="O47" s="83"/>
+      <c r="P47" s="83"/>
+      <c r="Q47" s="83"/>
+      <c r="R47" s="83"/>
+      <c r="S47" s="83"/>
+      <c r="T47" s="83"/>
+      <c r="U47" s="83"/>
+      <c r="V47" s="83"/>
+      <c r="W47" s="83"/>
+      <c r="X47" s="83"/>
+      <c r="Y47" s="83"/>
+      <c r="Z47" s="83"/>
+      <c r="AA47" s="83"/>
+      <c r="AB47" s="83"/>
+      <c r="AC47" s="83"/>
+      <c r="AD47" s="83"/>
+      <c r="AE47" s="83"/>
+      <c r="AF47" s="83"/>
+      <c r="AG47" s="83"/>
+      <c r="AH47" s="83"/>
+      <c r="AI47" s="83"/>
+      <c r="AJ47" s="83"/>
+      <c r="AK47" s="83"/>
+      <c r="AL47" s="83"/>
+      <c r="AM47" s="83"/>
+      <c r="AN47" s="83"/>
+      <c r="AO47" s="83"/>
+      <c r="AP47" s="83"/>
+      <c r="AQ47" s="83"/>
+      <c r="AR47" s="83"/>
+      <c r="AS47" s="83"/>
+      <c r="AT47" s="83"/>
+      <c r="AU47" s="83"/>
+      <c r="AV47" s="83"/>
+      <c r="AW47" s="83"/>
+      <c r="AX47" s="83"/>
+      <c r="AY47" s="83"/>
+      <c r="AZ47" s="83"/>
+      <c r="BA47" s="83"/>
+      <c r="BB47" s="83"/>
+      <c r="BC47" s="83"/>
+      <c r="BD47" s="83"/>
+      <c r="BE47" s="83"/>
+      <c r="BF47" s="83"/>
+      <c r="BG47" s="83"/>
+      <c r="BH47" s="83"/>
+      <c r="BI47" s="83"/>
+      <c r="BJ47" s="83"/>
+      <c r="BK47" s="83"/>
+      <c r="BL47" s="83"/>
+      <c r="BM47" s="83"/>
+      <c r="BN47" s="83"/>
+      <c r="BO47" s="83"/>
+      <c r="BP47" s="83"/>
+      <c r="BQ47" s="83"/>
+      <c r="BR47" s="83"/>
+      <c r="BS47" s="83"/>
+      <c r="BT47" s="83"/>
+      <c r="BU47" s="83"/>
+      <c r="BV47" s="83"/>
+      <c r="BW47" s="83"/>
+      <c r="BX47" s="83"/>
+      <c r="BY47" s="83"/>
+      <c r="BZ47" s="83"/>
+      <c r="CA47" s="83"/>
+      <c r="CB47" s="83"/>
+      <c r="CC47" s="83"/>
+      <c r="CD47" s="83"/>
+      <c r="CE47" s="83"/>
+      <c r="CF47" s="83"/>
+      <c r="CG47" s="83"/>
+      <c r="CH47" s="83"/>
+      <c r="CI47" s="83"/>
+      <c r="CJ47" s="83"/>
+      <c r="CK47" s="83"/>
+      <c r="CL47" s="83"/>
+      <c r="CM47" s="83"/>
+      <c r="CN47" s="83"/>
+      <c r="CO47" s="83"/>
+      <c r="CP47" s="83"/>
+      <c r="CQ47" s="83"/>
+      <c r="CR47" s="83"/>
+      <c r="CS47" s="83"/>
+      <c r="CT47" s="83"/>
+      <c r="CU47" s="83"/>
     </row>
     <row r="48" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="B48" s="100" t="s">
+      <c r="A48" s="6"/>
+      <c r="G48" s="6"/>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="17"/>
+      <c r="F49" s="96">
+        <v>43113</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="C48" s="18"/>
+      <c r="C50" s="18"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="99" t="s">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="99" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="CO4:CU4"/>
+    <mergeCell ref="J1:AA1"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="J1:AA1"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="BF4:BL4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="CO4:CU4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D45">
+  <conditionalFormatting sqref="D7:D47">
     <cfRule type="dataBar" priority="12">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -7019,7 +7244,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:CU45">
+  <conditionalFormatting sqref="I7:CU47">
     <cfRule type="expression" dxfId="2" priority="25">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -7027,7 +7252,7 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;I$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:CU45">
+  <conditionalFormatting sqref="I5:CU47">
     <cfRule type="expression" dxfId="0" priority="27">
       <formula>AND(today&gt;=I$5,today&lt;I$5+1)</formula>
     </cfRule>
@@ -7038,8 +7263,8 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B48" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B47" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B50" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B49" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="62" fitToHeight="0" orientation="landscape" r:id="rId3"/>
@@ -7061,7 +7286,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D45</xm:sqref>
+          <xm:sqref>D7:D47</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Javadoc export, documents folder order
</commit_message>
<xml_diff>
--- a/Documentation/Gantt_dia.xlsx
+++ b/Documentation/Gantt_dia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programok\2021\Git\EVP_Project\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6E0989-E362-4972-981E-E2C4BB499CE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39EC2E1-26D1-46E2-A056-79A1F304F385}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1078,6 +1078,9 @@
     <xf numFmtId="0" fontId="31" fillId="17" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1092,9 +1095,6 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1657,8 +1657,8 @@
   <dimension ref="A1:CU51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+      <pane ySplit="6" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1688,27 +1688,27 @@
       <c r="F1" s="97"/>
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
-      <c r="J1" s="115" t="str">
+      <c r="J1" s="110" t="str">
         <f>HYPERLINK("https://vertex42.link/HowToMakeAGanttChart","► Watch How to Make a Gantt Chart in Excel")</f>
         <v>► Watch How to Make a Gantt Chart in Excel</v>
       </c>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="115"/>
-      <c r="O1" s="115"/>
-      <c r="P1" s="115"/>
-      <c r="Q1" s="115"/>
-      <c r="R1" s="115"/>
-      <c r="S1" s="115"/>
-      <c r="T1" s="115"/>
-      <c r="U1" s="115"/>
-      <c r="V1" s="115"/>
-      <c r="W1" s="115"/>
-      <c r="X1" s="115"/>
-      <c r="Y1" s="115"/>
-      <c r="Z1" s="115"/>
-      <c r="AA1" s="115"/>
+      <c r="K1" s="110"/>
+      <c r="L1" s="110"/>
+      <c r="M1" s="110"/>
+      <c r="N1" s="110"/>
+      <c r="O1" s="110"/>
+      <c r="P1" s="110"/>
+      <c r="Q1" s="110"/>
+      <c r="R1" s="110"/>
+      <c r="S1" s="110"/>
+      <c r="T1" s="110"/>
+      <c r="U1" s="110"/>
+      <c r="V1" s="110"/>
+      <c r="W1" s="110"/>
+      <c r="X1" s="110"/>
+      <c r="Y1" s="110"/>
+      <c r="Z1" s="110"/>
+      <c r="AA1" s="110"/>
     </row>
     <row r="2" spans="1:99" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
@@ -1717,10 +1717,10 @@
       <c r="D2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="113">
+      <c r="E2" s="114">
         <v>44821</v>
       </c>
-      <c r="F2" s="114"/>
+      <c r="F2" s="115"/>
     </row>
     <row r="3" spans="1:99" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
@@ -1729,11 +1729,11 @@
       <c r="D3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="113">
+      <c r="E3" s="114">
         <f ca="1">TODAY()</f>
-        <v>44867</v>
-      </c>
-      <c r="F3" s="114"/>
+        <v>44930</v>
+      </c>
+      <c r="F3" s="115"/>
     </row>
     <row r="4" spans="1:99" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="6" t="s">
@@ -1742,136 +1742,136 @@
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="110">
+      <c r="I4" s="111">
         <f>I5</f>
         <v>44816</v>
       </c>
-      <c r="J4" s="111"/>
-      <c r="K4" s="111"/>
-      <c r="L4" s="111"/>
-      <c r="M4" s="111"/>
-      <c r="N4" s="111"/>
-      <c r="O4" s="112"/>
-      <c r="P4" s="110">
+      <c r="J4" s="112"/>
+      <c r="K4" s="112"/>
+      <c r="L4" s="112"/>
+      <c r="M4" s="112"/>
+      <c r="N4" s="112"/>
+      <c r="O4" s="113"/>
+      <c r="P4" s="111">
         <f>P5</f>
         <v>44823</v>
       </c>
-      <c r="Q4" s="111"/>
-      <c r="R4" s="111"/>
-      <c r="S4" s="111"/>
-      <c r="T4" s="111"/>
-      <c r="U4" s="111"/>
-      <c r="V4" s="112"/>
-      <c r="W4" s="110">
+      <c r="Q4" s="112"/>
+      <c r="R4" s="112"/>
+      <c r="S4" s="112"/>
+      <c r="T4" s="112"/>
+      <c r="U4" s="112"/>
+      <c r="V4" s="113"/>
+      <c r="W4" s="111">
         <f>W5</f>
         <v>44830</v>
       </c>
-      <c r="X4" s="111"/>
-      <c r="Y4" s="111"/>
-      <c r="Z4" s="111"/>
-      <c r="AA4" s="111"/>
-      <c r="AB4" s="111"/>
-      <c r="AC4" s="112"/>
-      <c r="AD4" s="110">
+      <c r="X4" s="112"/>
+      <c r="Y4" s="112"/>
+      <c r="Z4" s="112"/>
+      <c r="AA4" s="112"/>
+      <c r="AB4" s="112"/>
+      <c r="AC4" s="113"/>
+      <c r="AD4" s="111">
         <f>AD5</f>
         <v>44837</v>
       </c>
-      <c r="AE4" s="111"/>
-      <c r="AF4" s="111"/>
-      <c r="AG4" s="111"/>
-      <c r="AH4" s="111"/>
-      <c r="AI4" s="111"/>
-      <c r="AJ4" s="112"/>
-      <c r="AK4" s="110">
+      <c r="AE4" s="112"/>
+      <c r="AF4" s="112"/>
+      <c r="AG4" s="112"/>
+      <c r="AH4" s="112"/>
+      <c r="AI4" s="112"/>
+      <c r="AJ4" s="113"/>
+      <c r="AK4" s="111">
         <f>AK5</f>
         <v>44844</v>
       </c>
-      <c r="AL4" s="111"/>
-      <c r="AM4" s="111"/>
-      <c r="AN4" s="111"/>
-      <c r="AO4" s="111"/>
-      <c r="AP4" s="111"/>
-      <c r="AQ4" s="112"/>
-      <c r="AR4" s="110">
+      <c r="AL4" s="112"/>
+      <c r="AM4" s="112"/>
+      <c r="AN4" s="112"/>
+      <c r="AO4" s="112"/>
+      <c r="AP4" s="112"/>
+      <c r="AQ4" s="113"/>
+      <c r="AR4" s="111">
         <f>AR5</f>
         <v>44851</v>
       </c>
-      <c r="AS4" s="111"/>
-      <c r="AT4" s="111"/>
-      <c r="AU4" s="111"/>
-      <c r="AV4" s="111"/>
-      <c r="AW4" s="111"/>
-      <c r="AX4" s="112"/>
-      <c r="AY4" s="110">
+      <c r="AS4" s="112"/>
+      <c r="AT4" s="112"/>
+      <c r="AU4" s="112"/>
+      <c r="AV4" s="112"/>
+      <c r="AW4" s="112"/>
+      <c r="AX4" s="113"/>
+      <c r="AY4" s="111">
         <f>AY5</f>
         <v>44858</v>
       </c>
-      <c r="AZ4" s="111"/>
-      <c r="BA4" s="111"/>
-      <c r="BB4" s="111"/>
-      <c r="BC4" s="111"/>
-      <c r="BD4" s="111"/>
-      <c r="BE4" s="112"/>
-      <c r="BF4" s="110">
+      <c r="AZ4" s="112"/>
+      <c r="BA4" s="112"/>
+      <c r="BB4" s="112"/>
+      <c r="BC4" s="112"/>
+      <c r="BD4" s="112"/>
+      <c r="BE4" s="113"/>
+      <c r="BF4" s="111">
         <f>BF5</f>
         <v>44865</v>
       </c>
-      <c r="BG4" s="111"/>
-      <c r="BH4" s="111"/>
-      <c r="BI4" s="111"/>
-      <c r="BJ4" s="111"/>
-      <c r="BK4" s="111"/>
-      <c r="BL4" s="112"/>
-      <c r="BM4" s="110">
+      <c r="BG4" s="112"/>
+      <c r="BH4" s="112"/>
+      <c r="BI4" s="112"/>
+      <c r="BJ4" s="112"/>
+      <c r="BK4" s="112"/>
+      <c r="BL4" s="113"/>
+      <c r="BM4" s="111">
         <f>BM5</f>
         <v>44872</v>
       </c>
-      <c r="BN4" s="111"/>
-      <c r="BO4" s="111"/>
-      <c r="BP4" s="111"/>
-      <c r="BQ4" s="111"/>
-      <c r="BR4" s="111"/>
-      <c r="BS4" s="112"/>
-      <c r="BT4" s="110">
+      <c r="BN4" s="112"/>
+      <c r="BO4" s="112"/>
+      <c r="BP4" s="112"/>
+      <c r="BQ4" s="112"/>
+      <c r="BR4" s="112"/>
+      <c r="BS4" s="113"/>
+      <c r="BT4" s="111">
         <f>BT5</f>
         <v>44879</v>
       </c>
-      <c r="BU4" s="111"/>
-      <c r="BV4" s="111"/>
-      <c r="BW4" s="111"/>
-      <c r="BX4" s="111"/>
-      <c r="BY4" s="111"/>
-      <c r="BZ4" s="112"/>
-      <c r="CA4" s="110">
+      <c r="BU4" s="112"/>
+      <c r="BV4" s="112"/>
+      <c r="BW4" s="112"/>
+      <c r="BX4" s="112"/>
+      <c r="BY4" s="112"/>
+      <c r="BZ4" s="113"/>
+      <c r="CA4" s="111">
         <f>CA5</f>
         <v>44886</v>
       </c>
-      <c r="CB4" s="111"/>
-      <c r="CC4" s="111"/>
-      <c r="CD4" s="111"/>
-      <c r="CE4" s="111"/>
-      <c r="CF4" s="111"/>
-      <c r="CG4" s="112"/>
-      <c r="CH4" s="110">
+      <c r="CB4" s="112"/>
+      <c r="CC4" s="112"/>
+      <c r="CD4" s="112"/>
+      <c r="CE4" s="112"/>
+      <c r="CF4" s="112"/>
+      <c r="CG4" s="113"/>
+      <c r="CH4" s="111">
         <f>CH5</f>
         <v>44893</v>
       </c>
-      <c r="CI4" s="111"/>
-      <c r="CJ4" s="111"/>
-      <c r="CK4" s="111"/>
-      <c r="CL4" s="111"/>
-      <c r="CM4" s="111"/>
-      <c r="CN4" s="112"/>
-      <c r="CO4" s="110">
+      <c r="CI4" s="112"/>
+      <c r="CJ4" s="112"/>
+      <c r="CK4" s="112"/>
+      <c r="CL4" s="112"/>
+      <c r="CM4" s="112"/>
+      <c r="CN4" s="113"/>
+      <c r="CO4" s="111">
         <f>CO5</f>
         <v>44900</v>
       </c>
-      <c r="CP4" s="111"/>
-      <c r="CQ4" s="111"/>
-      <c r="CR4" s="111"/>
-      <c r="CS4" s="111"/>
-      <c r="CT4" s="111"/>
-      <c r="CU4" s="112"/>
+      <c r="CP4" s="112"/>
+      <c r="CQ4" s="112"/>
+      <c r="CR4" s="112"/>
+      <c r="CS4" s="112"/>
+      <c r="CT4" s="112"/>
+      <c r="CU4" s="113"/>
     </row>
     <row r="5" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
@@ -3750,7 +3750,7 @@
         <v>42</v>
       </c>
       <c r="D17" s="42">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="E17" s="43">
         <v>44849</v>
@@ -3864,18 +3864,18 @@
         <v>39</v>
       </c>
       <c r="D18" s="42">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E18" s="43">
         <v>44828</v>
       </c>
       <c r="F18" s="44">
-        <v>44896</v>
+        <v>44926</v>
       </c>
       <c r="G18" s="25"/>
       <c r="H18" s="25">
         <f t="shared" si="35"/>
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="I18" s="81"/>
       <c r="J18" s="81"/>
@@ -4302,7 +4302,7 @@
         <v>41</v>
       </c>
       <c r="D22" s="52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="53">
         <v>44862</v>
@@ -4416,7 +4416,7 @@
         <v>45</v>
       </c>
       <c r="D23" s="52">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E23" s="53">
         <v>44864</v>
@@ -4530,7 +4530,7 @@
         <v>42</v>
       </c>
       <c r="D24" s="52">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="E24" s="53">
         <v>44862</v>
@@ -4644,7 +4644,7 @@
         <v>39</v>
       </c>
       <c r="D25" s="52">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="E25" s="53">
         <v>44862</v>
@@ -4755,7 +4755,7 @@
         <v>39</v>
       </c>
       <c r="D26" s="52">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="E26" s="53">
         <v>44855</v>
@@ -4866,7 +4866,7 @@
         <v>42</v>
       </c>
       <c r="D27" s="52">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="E27" s="53">
         <v>44862</v>
@@ -5197,7 +5197,7 @@
         <v>41</v>
       </c>
       <c r="D30" s="62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="63">
         <v>44869</v>
@@ -5311,7 +5311,7 @@
         <v>45</v>
       </c>
       <c r="D31" s="62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" s="63">
         <v>44871</v>
@@ -5425,7 +5425,7 @@
         <v>42</v>
       </c>
       <c r="D32" s="62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" s="63">
         <v>44869</v>
@@ -5539,7 +5539,7 @@
         <v>42</v>
       </c>
       <c r="D33" s="62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" s="63">
         <v>44874</v>
@@ -5863,7 +5863,7 @@
         <v>41</v>
       </c>
       <c r="D36" s="72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36" s="73">
         <v>44876</v>
@@ -5977,7 +5977,7 @@
         <v>45</v>
       </c>
       <c r="D37" s="72">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="E37" s="73">
         <v>44878</v>
@@ -6091,7 +6091,7 @@
         <v>42</v>
       </c>
       <c r="D38" s="72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" s="73">
         <v>44876</v>
@@ -6205,7 +6205,7 @@
         <v>39</v>
       </c>
       <c r="D39" s="72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" s="73">
         <v>44883</v>
@@ -6539,7 +6539,7 @@
         <v>41</v>
       </c>
       <c r="D42" s="107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42" s="108">
         <v>44896</v>
@@ -6650,7 +6650,7 @@
         <v>45</v>
       </c>
       <c r="D43" s="107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43" s="108">
         <v>44898</v>
@@ -6761,7 +6761,7 @@
         <v>42</v>
       </c>
       <c r="D44" s="107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44" s="108">
         <v>44896</v>
@@ -6872,7 +6872,7 @@
         <v>42</v>
       </c>
       <c r="D45" s="107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E45" s="108">
         <v>44898</v>
@@ -7213,22 +7213,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="J1:AA1"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="BF4:BL4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="CO4:CU4"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="CO4:CU4"/>
+    <mergeCell ref="J1:AA1"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="BF4:BL4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D47">
     <cfRule type="dataBar" priority="12">
@@ -7267,7 +7267,7 @@
     <hyperlink ref="B49" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="62" fitToHeight="0" orientation="landscape" r:id="rId3"/>
+  <pageSetup scale="39" fitToHeight="0" orientation="landscape" r:id="rId3"/>
   <headerFooter scaleWithDoc="0"/>
   <legacyDrawing r:id="rId4"/>
   <extLst>

</xml_diff>